<commit_message>
address issue #5: Convert Excel date float into string for form processing. Adapt description in Excel templates.
</commit_message>
<xml_diff>
--- a/rotmic/static/uploadexample_cellsample.xlsx
+++ b/rotmic/static/uploadexample_cellsample.xlsx
@@ -16,7 +16,7 @@
     <definedName name="concentrationUnits">predefined!$C$5:$C$9</definedName>
     <definedName name="statusChoices">predefined!$A$5:$A$9</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="51">
   <si>
     <t>Description</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>prepared</t>
-  </si>
-  <si>
     <t>Concentration</t>
   </si>
   <si>
@@ -205,12 +202,21 @@
   </si>
   <si>
     <t>experiment #</t>
+  </si>
+  <si>
+    <t>14/03/2011</t>
+  </si>
+  <si>
+    <t>Prepared</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -298,7 +304,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -322,6 +328,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -397,12 +406,26 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Fields marked in </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Bold</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> are required. Rows without any value in the first column will be ignored.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Note, the preparation date needs to be formatted as shown in the example</a:t>
+            <a:t>Note, the preparation date can either be formatted as string '2014-01-28  or as proper Excel date.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -725,7 +748,7 @@
   <dimension ref="A1:O48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -748,7 +771,7 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -761,38 +784,38 @@
       <c r="C10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I10" s="8" t="s">
+      <c r="J10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L10" s="8" t="s">
+      <c r="M10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="N10" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>0</v>
@@ -800,654 +823,656 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>29</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L11" s="7">
         <v>250</v>
       </c>
       <c r="M11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N11" s="7">
         <v>5</v>
       </c>
       <c r="O11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>46</v>
+        <v>12</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="E12" s="11"/>
       <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" t="s">
         <v>42</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12" t="s">
-        <v>43</v>
       </c>
       <c r="L12" s="7">
         <v>400</v>
       </c>
       <c r="M12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="E13" s="11"/>
       <c r="H13" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="C14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D14" s="13"/>
       <c r="E14" s="11"/>
       <c r="H14" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="C15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D15" s="13"/>
       <c r="E15" s="11"/>
       <c r="H15" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D16" s="13"/>
       <c r="E16" s="11"/>
       <c r="H16" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="3:13">
       <c r="C17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D17" s="13"/>
       <c r="E17" s="11"/>
       <c r="H17" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="3:13">
       <c r="C18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D18" s="13"/>
       <c r="E18" s="11"/>
       <c r="H18" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="3:13">
       <c r="C19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D19" s="13"/>
       <c r="E19" s="11"/>
       <c r="H19" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="3:13">
       <c r="C20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D20" s="13"/>
       <c r="E20" s="11"/>
       <c r="H20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="3:13">
       <c r="C21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D21" s="13"/>
       <c r="E21" s="11"/>
       <c r="H21" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="3:13">
       <c r="C22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D22" s="13"/>
       <c r="E22" s="11"/>
       <c r="H22" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="3:13">
       <c r="C23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D23" s="13"/>
       <c r="E23" s="11"/>
       <c r="H23" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="3:13">
       <c r="C24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D24" s="13"/>
       <c r="E24" s="11"/>
       <c r="H24" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="3:13">
       <c r="C25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D25" s="13"/>
       <c r="E25" s="11"/>
       <c r="H25" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="3:13">
       <c r="C26" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D26" s="13"/>
       <c r="E26" s="11"/>
       <c r="H26" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="3:13">
       <c r="C27" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D27" s="13"/>
       <c r="E27" s="11"/>
       <c r="H27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="3:13">
       <c r="C28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D28" s="13"/>
       <c r="E28" s="11"/>
       <c r="H28" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="3:13">
       <c r="C29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D29" s="13"/>
       <c r="E29" s="11"/>
       <c r="H29" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="3:13">
       <c r="C30" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D30" s="13"/>
       <c r="E30" s="11"/>
       <c r="H30" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="3:13">
       <c r="C31" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D31" s="13"/>
       <c r="E31" s="11"/>
       <c r="H31" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="3:13">
       <c r="C32" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D32" s="13"/>
       <c r="E32" s="11"/>
       <c r="H32" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="3:13">
       <c r="C33" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D33" s="13"/>
       <c r="E33" s="11"/>
       <c r="H33" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="3:13">
       <c r="C34" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D34" s="13"/>
       <c r="E34" s="11"/>
       <c r="H34" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="3:13">
       <c r="C35" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D35" s="13"/>
       <c r="E35" s="11"/>
       <c r="H35" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="3:13">
       <c r="C36" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D36" s="13"/>
       <c r="E36" s="11"/>
       <c r="H36" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="3:13">
       <c r="C37" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D37" s="13"/>
       <c r="E37" s="11"/>
       <c r="H37" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="3:13">
       <c r="C38" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D38" s="13"/>
       <c r="E38" s="11"/>
       <c r="H38" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="3:13">
       <c r="C39" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D39" s="13"/>
       <c r="E39" s="11"/>
       <c r="H39" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="3:13">
       <c r="C40" t="s">
-        <v>13</v>
-      </c>
-      <c r="D40" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D40" s="13"/>
       <c r="E40" s="11"/>
       <c r="H40" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="3:13">
       <c r="C41" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D41" s="13"/>
       <c r="E41" s="11"/>
       <c r="H41" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="3:13">
       <c r="C42" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D42" s="13"/>
       <c r="E42" s="11"/>
       <c r="H42" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="3:13">
       <c r="C43" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D43" s="13"/>
       <c r="E43" s="11"/>
       <c r="H43" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J43" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="3:13">
       <c r="C44" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D44" s="13"/>
       <c r="E44" s="11"/>
       <c r="H44" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="3:13">
       <c r="C45" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D45" s="13"/>
       <c r="E45" s="11"/>
       <c r="H45" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="3:13">
       <c r="C46" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D46" s="13"/>
       <c r="E46" s="11"/>
       <c r="H46" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="3:13">
       <c r="C47" t="s">
-        <v>13</v>
-      </c>
-      <c r="D47" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D47" s="13"/>
       <c r="E47" s="11"/>
       <c r="H47" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="3:13">
       <c r="C48" t="s">
-        <v>13</v>
-      </c>
-      <c r="D48" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D48" s="13"/>
       <c r="E48" s="11"/>
       <c r="H48" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1507,13 +1532,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K4" t="s">
         <v>3</v>
@@ -1521,16 +1546,16 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L5" t="s">
         <v>3</v>
@@ -1538,16 +1563,16 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L6" t="s">
         <v>3</v>
@@ -1555,16 +1580,16 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L7" t="s">
         <v>3</v>
@@ -1572,16 +1597,16 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L8" t="s">
         <v>3</v>
@@ -1589,13 +1614,13 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L9" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
preparedBy support in upload tables. Autogeneration if left empty.
</commit_message>
<xml_diff>
--- a/rotmic/static/uploadexample_cellsample.xlsx
+++ b/rotmic/static/uploadexample_cellsample.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="53">
   <si>
     <t>Description</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>Prepared</t>
+  </si>
+  <si>
+    <t>By</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -215,9 +221,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,6 +273,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -304,7 +316,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -330,7 +342,10 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -353,7 +368,7 @@
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -427,6 +442,17 @@
             <a:rPr lang="en-US" sz="1100"/>
             <a:t>Note, the preparation date can either be formatted as string '2014-01-28  or as proper Excel date.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>By:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> refers to the user who prepared this sample. It has to be an exact rotmic user name. Leave empty to register the user uploading the table as "prepared By".</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1100"/>
@@ -745,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O48"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -756,25 +782,25 @@
     <col min="1" max="1" width="8.28515625" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="5" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="12" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="7" customWidth="1"/>
-    <col min="6" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="24" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" style="7" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" style="7" customWidth="1"/>
-    <col min="15" max="15" width="41" customWidth="1"/>
+    <col min="4" max="5" width="12" style="7" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="7" customWidth="1"/>
+    <col min="7" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" style="7" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" style="7" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" style="7" customWidth="1"/>
+    <col min="16" max="16" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:16">
       <c r="A10" s="9" t="s">
         <v>4</v>
       </c>
@@ -787,41 +813,44 @@
       <c r="D10" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="H10" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="I10" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="J10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L10" s="8" t="s">
+      <c r="M10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N10" s="8" t="s">
+      <c r="O10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -834,34 +863,35 @@
       <c r="D11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="3" t="s">
+      <c r="E11" s="13"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J11" t="s">
-        <v>18</v>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="K11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" t="s">
         <v>43</v>
       </c>
-      <c r="L11" s="7">
+      <c r="M11" s="7">
         <v>250</v>
       </c>
-      <c r="M11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N11" s="7">
+      <c r="N11" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" s="7">
         <v>5</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -874,619 +904,658 @@
       <c r="D12" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="G12" t="s">
+      <c r="E12" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="H12" t="s">
         <v>41</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J12" t="s">
-        <v>18</v>
-      </c>
       <c r="K12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" t="s">
         <v>42</v>
       </c>
-      <c r="L12" s="7">
+      <c r="M12" s="7">
         <v>400</v>
       </c>
-      <c r="M12" t="s">
-        <v>22</v>
-      </c>
-      <c r="O12" t="s">
+      <c r="N12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16">
       <c r="C13" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="H13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J13" t="s">
-        <v>18</v>
-      </c>
-      <c r="M13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="E13" s="13"/>
+      <c r="F13" s="11"/>
+      <c r="I13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="C14" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="13"/>
-      <c r="E14" s="11"/>
-      <c r="H14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J14" t="s">
-        <v>18</v>
-      </c>
-      <c r="M14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="E14" s="13"/>
+      <c r="F14" s="11"/>
+      <c r="I14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="C15" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="13"/>
-      <c r="E15" s="11"/>
-      <c r="H15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J15" t="s">
-        <v>18</v>
-      </c>
-      <c r="M15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="E15" s="13"/>
+      <c r="F15" s="11"/>
+      <c r="I15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="C16" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="13"/>
-      <c r="E16" s="11"/>
-      <c r="H16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J16" t="s">
-        <v>18</v>
-      </c>
-      <c r="M16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="3:13">
+      <c r="E16" s="13"/>
+      <c r="F16" s="11"/>
+      <c r="I16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K16" t="s">
+        <v>18</v>
+      </c>
+      <c r="N16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="3:14">
       <c r="C17" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="13"/>
-      <c r="E17" s="11"/>
-      <c r="H17" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J17" t="s">
-        <v>18</v>
-      </c>
-      <c r="M17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="3:13">
+      <c r="E17" s="13"/>
+      <c r="F17" s="11"/>
+      <c r="I17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K17" t="s">
+        <v>18</v>
+      </c>
+      <c r="N17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="3:14">
       <c r="C18" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="13"/>
-      <c r="E18" s="11"/>
-      <c r="H18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J18" t="s">
-        <v>18</v>
-      </c>
-      <c r="M18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="3:13">
+      <c r="E18" s="13"/>
+      <c r="F18" s="11"/>
+      <c r="I18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" t="s">
+        <v>18</v>
+      </c>
+      <c r="N18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14">
       <c r="C19" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="13"/>
-      <c r="E19" s="11"/>
-      <c r="H19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J19" t="s">
-        <v>18</v>
-      </c>
-      <c r="M19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="3:13">
+      <c r="E19" s="13"/>
+      <c r="F19" s="11"/>
+      <c r="I19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" t="s">
+        <v>18</v>
+      </c>
+      <c r="N19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="3:14">
       <c r="C20" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="13"/>
-      <c r="E20" s="11"/>
-      <c r="H20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J20" t="s">
-        <v>18</v>
-      </c>
-      <c r="M20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="3:13">
+      <c r="E20" s="13"/>
+      <c r="F20" s="11"/>
+      <c r="I20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" t="s">
+        <v>18</v>
+      </c>
+      <c r="N20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="3:14">
       <c r="C21" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="13"/>
-      <c r="E21" s="11"/>
-      <c r="H21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J21" t="s">
-        <v>18</v>
-      </c>
-      <c r="M21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="3:13">
+      <c r="E21" s="13"/>
+      <c r="F21" s="11"/>
+      <c r="I21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K21" t="s">
+        <v>18</v>
+      </c>
+      <c r="N21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="3:14">
       <c r="C22" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="13"/>
-      <c r="E22" s="11"/>
-      <c r="H22" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J22" t="s">
-        <v>18</v>
-      </c>
-      <c r="M22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="3:13">
+      <c r="E22" s="13"/>
+      <c r="F22" s="11"/>
+      <c r="I22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K22" t="s">
+        <v>18</v>
+      </c>
+      <c r="N22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="3:14">
       <c r="C23" t="s">
         <v>12</v>
       </c>
       <c r="D23" s="13"/>
-      <c r="E23" s="11"/>
-      <c r="H23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J23" t="s">
-        <v>18</v>
-      </c>
-      <c r="M23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="3:13">
+      <c r="E23" s="13"/>
+      <c r="F23" s="11"/>
+      <c r="I23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K23" t="s">
+        <v>18</v>
+      </c>
+      <c r="N23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="3:14">
       <c r="C24" t="s">
         <v>12</v>
       </c>
       <c r="D24" s="13"/>
-      <c r="E24" s="11"/>
-      <c r="H24" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J24" t="s">
-        <v>18</v>
-      </c>
-      <c r="M24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="3:13">
+      <c r="E24" s="13"/>
+      <c r="F24" s="11"/>
+      <c r="I24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K24" t="s">
+        <v>18</v>
+      </c>
+      <c r="N24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="3:14">
       <c r="C25" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="13"/>
-      <c r="E25" s="11"/>
-      <c r="H25" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J25" t="s">
-        <v>18</v>
-      </c>
-      <c r="M25" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="3:13">
+      <c r="E25" s="13"/>
+      <c r="F25" s="11"/>
+      <c r="I25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K25" t="s">
+        <v>18</v>
+      </c>
+      <c r="N25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="3:14">
       <c r="C26" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="13"/>
-      <c r="E26" s="11"/>
-      <c r="H26" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J26" t="s">
-        <v>18</v>
-      </c>
-      <c r="M26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="3:13">
+      <c r="E26" s="13"/>
+      <c r="F26" s="11"/>
+      <c r="I26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K26" t="s">
+        <v>18</v>
+      </c>
+      <c r="N26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="3:14">
       <c r="C27" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="13"/>
-      <c r="E27" s="11"/>
-      <c r="H27" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J27" t="s">
-        <v>18</v>
-      </c>
-      <c r="M27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="3:13">
+      <c r="E27" s="13"/>
+      <c r="F27" s="11"/>
+      <c r="I27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K27" t="s">
+        <v>18</v>
+      </c>
+      <c r="N27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="3:14">
       <c r="C28" t="s">
         <v>12</v>
       </c>
       <c r="D28" s="13"/>
-      <c r="E28" s="11"/>
-      <c r="H28" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J28" t="s">
-        <v>18</v>
-      </c>
-      <c r="M28" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="3:13">
+      <c r="E28" s="13"/>
+      <c r="F28" s="11"/>
+      <c r="I28" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K28" t="s">
+        <v>18</v>
+      </c>
+      <c r="N28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="3:14">
       <c r="C29" t="s">
         <v>12</v>
       </c>
       <c r="D29" s="13"/>
-      <c r="E29" s="11"/>
-      <c r="H29" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J29" t="s">
-        <v>18</v>
-      </c>
-      <c r="M29" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="3:13">
+      <c r="E29" s="13"/>
+      <c r="F29" s="11"/>
+      <c r="I29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K29" t="s">
+        <v>18</v>
+      </c>
+      <c r="N29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="3:14">
       <c r="C30" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="13"/>
-      <c r="E30" s="11"/>
-      <c r="H30" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J30" t="s">
-        <v>18</v>
-      </c>
-      <c r="M30" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="3:13">
+      <c r="E30" s="13"/>
+      <c r="F30" s="11"/>
+      <c r="I30" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K30" t="s">
+        <v>18</v>
+      </c>
+      <c r="N30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="3:14">
       <c r="C31" t="s">
         <v>12</v>
       </c>
       <c r="D31" s="13"/>
-      <c r="E31" s="11"/>
-      <c r="H31" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J31" t="s">
-        <v>18</v>
-      </c>
-      <c r="M31" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="3:13">
+      <c r="E31" s="13"/>
+      <c r="F31" s="11"/>
+      <c r="I31" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K31" t="s">
+        <v>18</v>
+      </c>
+      <c r="N31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="3:14">
       <c r="C32" t="s">
         <v>12</v>
       </c>
       <c r="D32" s="13"/>
-      <c r="E32" s="11"/>
-      <c r="H32" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J32" t="s">
-        <v>18</v>
-      </c>
-      <c r="M32" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="3:13">
+      <c r="E32" s="13"/>
+      <c r="F32" s="11"/>
+      <c r="I32" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K32" t="s">
+        <v>18</v>
+      </c>
+      <c r="N32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="3:14">
       <c r="C33" t="s">
         <v>12</v>
       </c>
       <c r="D33" s="13"/>
-      <c r="E33" s="11"/>
-      <c r="H33" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J33" t="s">
-        <v>18</v>
-      </c>
-      <c r="M33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="3:13">
+      <c r="E33" s="13"/>
+      <c r="F33" s="11"/>
+      <c r="I33" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K33" t="s">
+        <v>18</v>
+      </c>
+      <c r="N33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="3:14">
       <c r="C34" t="s">
         <v>12</v>
       </c>
       <c r="D34" s="13"/>
-      <c r="E34" s="11"/>
-      <c r="H34" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J34" t="s">
-        <v>18</v>
-      </c>
-      <c r="M34" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="3:13">
+      <c r="E34" s="13"/>
+      <c r="F34" s="11"/>
+      <c r="I34" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K34" t="s">
+        <v>18</v>
+      </c>
+      <c r="N34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="3:14">
       <c r="C35" t="s">
         <v>12</v>
       </c>
       <c r="D35" s="13"/>
-      <c r="E35" s="11"/>
-      <c r="H35" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J35" t="s">
-        <v>18</v>
-      </c>
-      <c r="M35" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="36" spans="3:13">
+      <c r="E35" s="13"/>
+      <c r="F35" s="11"/>
+      <c r="I35" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K35" t="s">
+        <v>18</v>
+      </c>
+      <c r="N35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="3:14">
       <c r="C36" t="s">
         <v>12</v>
       </c>
       <c r="D36" s="13"/>
-      <c r="E36" s="11"/>
-      <c r="H36" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J36" t="s">
-        <v>18</v>
-      </c>
-      <c r="M36" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="3:13">
+      <c r="E36" s="13"/>
+      <c r="F36" s="11"/>
+      <c r="I36" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K36" t="s">
+        <v>18</v>
+      </c>
+      <c r="N36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="3:14">
       <c r="C37" t="s">
         <v>12</v>
       </c>
       <c r="D37" s="13"/>
-      <c r="E37" s="11"/>
-      <c r="H37" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J37" t="s">
-        <v>18</v>
-      </c>
-      <c r="M37" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="38" spans="3:13">
+      <c r="E37" s="13"/>
+      <c r="F37" s="11"/>
+      <c r="I37" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K37" t="s">
+        <v>18</v>
+      </c>
+      <c r="N37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="3:14">
       <c r="C38" t="s">
         <v>12</v>
       </c>
       <c r="D38" s="13"/>
-      <c r="E38" s="11"/>
-      <c r="H38" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J38" t="s">
-        <v>18</v>
-      </c>
-      <c r="M38" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="39" spans="3:13">
+      <c r="E38" s="13"/>
+      <c r="F38" s="11"/>
+      <c r="I38" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K38" t="s">
+        <v>18</v>
+      </c>
+      <c r="N38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="3:14">
       <c r="C39" t="s">
         <v>12</v>
       </c>
       <c r="D39" s="13"/>
-      <c r="E39" s="11"/>
-      <c r="H39" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J39" t="s">
-        <v>18</v>
-      </c>
-      <c r="M39" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" spans="3:13">
+      <c r="E39" s="13"/>
+      <c r="F39" s="11"/>
+      <c r="I39" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K39" t="s">
+        <v>18</v>
+      </c>
+      <c r="N39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="3:14">
       <c r="C40" t="s">
         <v>12</v>
       </c>
       <c r="D40" s="13"/>
-      <c r="E40" s="11"/>
-      <c r="H40" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J40" t="s">
-        <v>18</v>
-      </c>
-      <c r="M40" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="41" spans="3:13">
+      <c r="E40" s="13"/>
+      <c r="F40" s="11"/>
+      <c r="I40" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K40" t="s">
+        <v>18</v>
+      </c>
+      <c r="N40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="3:14">
       <c r="C41" t="s">
         <v>12</v>
       </c>
       <c r="D41" s="13"/>
-      <c r="E41" s="11"/>
-      <c r="H41" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J41" t="s">
-        <v>18</v>
-      </c>
-      <c r="M41" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="42" spans="3:13">
+      <c r="E41" s="13"/>
+      <c r="F41" s="11"/>
+      <c r="I41" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K41" t="s">
+        <v>18</v>
+      </c>
+      <c r="N41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="3:14">
       <c r="C42" t="s">
         <v>12</v>
       </c>
       <c r="D42" s="13"/>
-      <c r="E42" s="11"/>
-      <c r="H42" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J42" t="s">
-        <v>18</v>
-      </c>
-      <c r="M42" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="3:13">
+      <c r="E42" s="13"/>
+      <c r="F42" s="11"/>
+      <c r="I42" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K42" t="s">
+        <v>18</v>
+      </c>
+      <c r="N42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="3:14">
       <c r="C43" t="s">
         <v>12</v>
       </c>
       <c r="D43" s="13"/>
-      <c r="E43" s="11"/>
-      <c r="H43" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J43" t="s">
-        <v>18</v>
-      </c>
-      <c r="M43" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44" spans="3:13">
+      <c r="E43" s="13"/>
+      <c r="F43" s="11"/>
+      <c r="I43" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K43" t="s">
+        <v>18</v>
+      </c>
+      <c r="N43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="3:14">
       <c r="C44" t="s">
         <v>12</v>
       </c>
       <c r="D44" s="13"/>
-      <c r="E44" s="11"/>
-      <c r="H44" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J44" t="s">
-        <v>18</v>
-      </c>
-      <c r="M44" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" spans="3:13">
+      <c r="E44" s="13"/>
+      <c r="F44" s="11"/>
+      <c r="I44" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K44" t="s">
+        <v>18</v>
+      </c>
+      <c r="N44" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="3:14">
       <c r="C45" t="s">
         <v>12</v>
       </c>
       <c r="D45" s="13"/>
-      <c r="E45" s="11"/>
-      <c r="H45" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J45" t="s">
-        <v>18</v>
-      </c>
-      <c r="M45" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="3:13">
+      <c r="E45" s="13"/>
+      <c r="F45" s="11"/>
+      <c r="I45" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K45" t="s">
+        <v>18</v>
+      </c>
+      <c r="N45" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="3:14">
       <c r="C46" t="s">
         <v>12</v>
       </c>
       <c r="D46" s="13"/>
-      <c r="E46" s="11"/>
-      <c r="H46" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J46" t="s">
-        <v>18</v>
-      </c>
-      <c r="M46" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" spans="3:13">
+      <c r="E46" s="13"/>
+      <c r="F46" s="11"/>
+      <c r="I46" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K46" t="s">
+        <v>18</v>
+      </c>
+      <c r="N46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="3:14">
       <c r="C47" t="s">
         <v>12</v>
       </c>
       <c r="D47" s="13"/>
-      <c r="E47" s="11"/>
-      <c r="H47" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J47" t="s">
-        <v>18</v>
-      </c>
-      <c r="M47" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="3:13">
+      <c r="E47" s="13"/>
+      <c r="F47" s="11"/>
+      <c r="I47" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K47" t="s">
+        <v>18</v>
+      </c>
+      <c r="N47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="3:14">
       <c r="C48" t="s">
         <v>12</v>
       </c>
       <c r="D48" s="13"/>
-      <c r="E48" s="11"/>
-      <c r="H48" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J48" t="s">
-        <v>18</v>
-      </c>
-      <c r="M48" t="s">
+      <c r="E48" s="13"/>
+      <c r="F48" s="11"/>
+      <c r="I48" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K48" t="s">
+        <v>18</v>
+      </c>
+      <c r="N48" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J11:J48">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="K11:K48">
       <formula1>concentrationUnits</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M11:M48">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N11:N48">
       <formula1>amountUnits</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C48">
       <formula1>statusChoices</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H11:H48">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I11:I48">
       <formula1>cellChoices</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
correct column Aliquotes -> Aliquots
</commit_message>
<xml_diff>
--- a/rotmic/static/uploadexample_cellsample.xlsx
+++ b/rotmic/static/uploadexample_cellsample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5790" yWindow="30" windowWidth="26265" windowHeight="15390"/>
+    <workbookView xWindow="5790" yWindow="30" windowWidth="25860" windowHeight="15390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -132,9 +132,6 @@
     <t>L</t>
   </si>
   <si>
-    <t>Aliquotes</t>
-  </si>
-  <si>
     <t>test sample</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>Aliquots</t>
   </si>
 </sst>
 </file>
@@ -774,7 +774,7 @@
   <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -797,7 +797,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -811,22 +811,22 @@
         <v>6</v>
       </c>
       <c r="D10" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>51</v>
-      </c>
       <c r="F10" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>7</v>
@@ -844,7 +844,7 @@
         <v>11</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>0</v>
@@ -852,31 +852,31 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>28</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="11"/>
       <c r="G11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K11" t="s">
         <v>18</v>
       </c>
       <c r="L11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M11" s="7">
         <v>250</v>
@@ -888,37 +888,37 @@
         <v>5</v>
       </c>
       <c r="P11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F12" s="11"/>
       <c r="H12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" t="s">
         <v>41</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K12" t="s">
-        <v>18</v>
-      </c>
-      <c r="L12" t="s">
-        <v>42</v>
       </c>
       <c r="M12" s="7">
         <v>400</v>
@@ -927,7 +927,7 @@
         <v>22</v>
       </c>
       <c r="P12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -935,12 +935,12 @@
         <v>12</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="11"/>
       <c r="I13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K13" t="s">
         <v>18</v>
@@ -957,7 +957,7 @@
       <c r="E14" s="13"/>
       <c r="F14" s="11"/>
       <c r="I14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K14" t="s">
         <v>18</v>
@@ -974,7 +974,7 @@
       <c r="E15" s="13"/>
       <c r="F15" s="11"/>
       <c r="I15" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K15" t="s">
         <v>18</v>
@@ -991,7 +991,7 @@
       <c r="E16" s="13"/>
       <c r="F16" s="11"/>
       <c r="I16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K16" t="s">
         <v>18</v>
@@ -1008,7 +1008,7 @@
       <c r="E17" s="13"/>
       <c r="F17" s="11"/>
       <c r="I17" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K17" t="s">
         <v>18</v>
@@ -1025,7 +1025,7 @@
       <c r="E18" s="13"/>
       <c r="F18" s="11"/>
       <c r="I18" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K18" t="s">
         <v>18</v>
@@ -1042,7 +1042,7 @@
       <c r="E19" s="13"/>
       <c r="F19" s="11"/>
       <c r="I19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K19" t="s">
         <v>18</v>
@@ -1059,7 +1059,7 @@
       <c r="E20" s="13"/>
       <c r="F20" s="11"/>
       <c r="I20" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K20" t="s">
         <v>18</v>
@@ -1076,7 +1076,7 @@
       <c r="E21" s="13"/>
       <c r="F21" s="11"/>
       <c r="I21" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K21" t="s">
         <v>18</v>
@@ -1093,7 +1093,7 @@
       <c r="E22" s="13"/>
       <c r="F22" s="11"/>
       <c r="I22" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K22" t="s">
         <v>18</v>
@@ -1110,7 +1110,7 @@
       <c r="E23" s="13"/>
       <c r="F23" s="11"/>
       <c r="I23" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K23" t="s">
         <v>18</v>
@@ -1127,7 +1127,7 @@
       <c r="E24" s="13"/>
       <c r="F24" s="11"/>
       <c r="I24" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K24" t="s">
         <v>18</v>
@@ -1144,7 +1144,7 @@
       <c r="E25" s="13"/>
       <c r="F25" s="11"/>
       <c r="I25" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K25" t="s">
         <v>18</v>
@@ -1161,7 +1161,7 @@
       <c r="E26" s="13"/>
       <c r="F26" s="11"/>
       <c r="I26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K26" t="s">
         <v>18</v>
@@ -1178,7 +1178,7 @@
       <c r="E27" s="13"/>
       <c r="F27" s="11"/>
       <c r="I27" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K27" t="s">
         <v>18</v>
@@ -1195,7 +1195,7 @@
       <c r="E28" s="13"/>
       <c r="F28" s="11"/>
       <c r="I28" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K28" t="s">
         <v>18</v>
@@ -1212,7 +1212,7 @@
       <c r="E29" s="13"/>
       <c r="F29" s="11"/>
       <c r="I29" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K29" t="s">
         <v>18</v>
@@ -1229,7 +1229,7 @@
       <c r="E30" s="13"/>
       <c r="F30" s="11"/>
       <c r="I30" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K30" t="s">
         <v>18</v>
@@ -1246,7 +1246,7 @@
       <c r="E31" s="13"/>
       <c r="F31" s="11"/>
       <c r="I31" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K31" t="s">
         <v>18</v>
@@ -1263,7 +1263,7 @@
       <c r="E32" s="13"/>
       <c r="F32" s="11"/>
       <c r="I32" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K32" t="s">
         <v>18</v>
@@ -1280,7 +1280,7 @@
       <c r="E33" s="13"/>
       <c r="F33" s="11"/>
       <c r="I33" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K33" t="s">
         <v>18</v>
@@ -1297,7 +1297,7 @@
       <c r="E34" s="13"/>
       <c r="F34" s="11"/>
       <c r="I34" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K34" t="s">
         <v>18</v>
@@ -1314,7 +1314,7 @@
       <c r="E35" s="13"/>
       <c r="F35" s="11"/>
       <c r="I35" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K35" t="s">
         <v>18</v>
@@ -1331,7 +1331,7 @@
       <c r="E36" s="13"/>
       <c r="F36" s="11"/>
       <c r="I36" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K36" t="s">
         <v>18</v>
@@ -1348,7 +1348,7 @@
       <c r="E37" s="13"/>
       <c r="F37" s="11"/>
       <c r="I37" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K37" t="s">
         <v>18</v>
@@ -1365,7 +1365,7 @@
       <c r="E38" s="13"/>
       <c r="F38" s="11"/>
       <c r="I38" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K38" t="s">
         <v>18</v>
@@ -1382,7 +1382,7 @@
       <c r="E39" s="13"/>
       <c r="F39" s="11"/>
       <c r="I39" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K39" t="s">
         <v>18</v>
@@ -1399,7 +1399,7 @@
       <c r="E40" s="13"/>
       <c r="F40" s="11"/>
       <c r="I40" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K40" t="s">
         <v>18</v>
@@ -1416,7 +1416,7 @@
       <c r="E41" s="13"/>
       <c r="F41" s="11"/>
       <c r="I41" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K41" t="s">
         <v>18</v>
@@ -1433,7 +1433,7 @@
       <c r="E42" s="13"/>
       <c r="F42" s="11"/>
       <c r="I42" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K42" t="s">
         <v>18</v>
@@ -1450,7 +1450,7 @@
       <c r="E43" s="13"/>
       <c r="F43" s="11"/>
       <c r="I43" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K43" t="s">
         <v>18</v>
@@ -1467,7 +1467,7 @@
       <c r="E44" s="13"/>
       <c r="F44" s="11"/>
       <c r="I44" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K44" t="s">
         <v>18</v>
@@ -1484,7 +1484,7 @@
       <c r="E45" s="13"/>
       <c r="F45" s="11"/>
       <c r="I45" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K45" t="s">
         <v>18</v>
@@ -1501,7 +1501,7 @@
       <c r="E46" s="13"/>
       <c r="F46" s="11"/>
       <c r="I46" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K46" t="s">
         <v>18</v>
@@ -1518,7 +1518,7 @@
       <c r="E47" s="13"/>
       <c r="F47" s="11"/>
       <c r="I47" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K47" t="s">
         <v>18</v>
@@ -1535,7 +1535,7 @@
       <c r="E48" s="13"/>
       <c r="F48" s="11"/>
       <c r="I48" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K48" t="s">
         <v>18</v>
@@ -1607,7 +1607,7 @@
         <v>11</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K4" t="s">
         <v>3</v>
@@ -1624,7 +1624,7 @@
         <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L5" t="s">
         <v>3</v>
@@ -1641,7 +1641,7 @@
         <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L6" t="s">
         <v>3</v>
@@ -1658,7 +1658,7 @@
         <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L7" t="s">
         <v>3</v>
@@ -1672,10 +1672,10 @@
         <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L8" t="s">
         <v>3</v>
@@ -1689,7 +1689,7 @@
         <v>21</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L9" t="s">
         <v>3</v>

</xml_diff>